<commit_message>
updated e2e testing, changed testing spreadsheets to values greater than 1000000 to signify testing data
</commit_message>
<xml_diff>
--- a/feedback_forms/testing_versions/standard/dairy_digester_operator_feedback_v006_test_01_good_data.xlsx
+++ b/feedback_forms/testing_versions/standard/dairy_digester_operator_feedback_v006_test_01_good_data.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tony_local\pycharm\feedback_portal\feedback_forms\testing_versions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\local\cursor\feedback_portal\feedback_forms\testing_versions\standard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3175EB35-B875-4340-898C-C910733C0163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655750F0-5FFB-4AC5-9462-886722AB6D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ZZdeBZIs3h22LxegpdwwuHpsWEWuB9x+vvy4q5aW62Xkr4aTJmE005hpcsO5kgTp7rwoerT5PSsZglAASxcSXg==" workbookSaltValue="WgC7rnmlwtCTlwVo9LJMCQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3247" yWindow="680" windowWidth="19200" windowHeight="11387" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="6840" yWindow="4491" windowWidth="21729" windowHeight="13260" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
@@ -3772,26 +3772,26 @@
   <dimension ref="B1:G97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.1171875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="65.703125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="4.703125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="65.703125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="4.1171875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="4.07421875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="65.69140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="4.69140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="65.69140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="4.07421875" style="9" customWidth="1"/>
     <col min="6" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
       <c r="E1" s="32"/>
     </row>
-    <row r="2" spans="2:5" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:5" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.4">
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
@@ -3799,7 +3799,7 @@
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="2:5" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:5" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.4">
       <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
@@ -3807,26 +3807,26 @@
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="2:5" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:5" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
       <c r="E4" s="37"/>
     </row>
-    <row r="5" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
       <c r="E5" s="32"/>
     </row>
-    <row r="6" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:5" s="40" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="39"/>
     </row>
-    <row r="7" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="8" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B8" s="41" t="s">
         <v>2</v>
       </c>
@@ -3834,7 +3834,7 @@
       <c r="D8" s="42"/>
       <c r="E8" s="42"/>
     </row>
-    <row r="9" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B9" s="44" t="s">
         <v>3</v>
       </c>
@@ -3842,7 +3842,7 @@
       <c r="D9" s="45"/>
       <c r="E9" s="42"/>
     </row>
-    <row r="10" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B10" s="46" t="s">
         <v>4</v>
       </c>
@@ -3850,7 +3850,7 @@
       <c r="D10" s="47"/>
       <c r="E10" s="42"/>
     </row>
-    <row r="11" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B11" s="41" t="s">
         <v>5</v>
       </c>
@@ -3858,7 +3858,7 @@
       <c r="D11" s="42"/>
       <c r="E11" s="42"/>
     </row>
-    <row r="12" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B12" s="41" t="s">
         <v>6</v>
       </c>
@@ -3866,7 +3866,7 @@
       <c r="D12" s="42"/>
       <c r="E12" s="42"/>
     </row>
-    <row r="13" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B13" s="41" t="s">
         <v>7</v>
       </c>
@@ -3874,7 +3874,7 @@
       <c r="D13" s="42"/>
       <c r="E13" s="42"/>
     </row>
-    <row r="14" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B14" s="41" t="s">
         <v>8</v>
       </c>
@@ -3882,7 +3882,7 @@
       <c r="D14" s="42"/>
       <c r="E14" s="42"/>
     </row>
-    <row r="15" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B15" s="48" t="s">
         <v>9</v>
       </c>
@@ -3890,7 +3890,7 @@
       <c r="D15" s="49"/>
       <c r="E15" s="49"/>
     </row>
-    <row r="16" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B16" s="41" t="s">
         <v>10</v>
       </c>
@@ -3898,7 +3898,7 @@
       <c r="D16" s="42"/>
       <c r="E16" s="42"/>
     </row>
-    <row r="17" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B17" s="41" t="s">
         <v>11</v>
       </c>
@@ -3906,25 +3906,25 @@
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
     </row>
-    <row r="18" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="19" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="2:5" s="40" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
       <c r="D19" s="38"/>
       <c r="E19" s="39"/>
     </row>
-    <row r="20" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="21" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B21" s="41" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="61">
-        <v>2001</v>
+        <v>1002001</v>
       </c>
       <c r="E21" s="41"/>
     </row>
-    <row r="22" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B22" s="41" t="s">
         <v>13</v>
       </c>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="E22" s="42"/>
     </row>
-    <row r="23" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:5" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B23" s="41" t="s">
         <v>14</v>
       </c>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="E23" s="42"/>
     </row>
-    <row r="24" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B24" s="41" t="s">
         <v>15</v>
       </c>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="E24" s="41"/>
     </row>
-    <row r="25" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B25" s="41" t="s">
         <v>16</v>
       </c>
@@ -3964,7 +3964,7 @@
       </c>
       <c r="E25" s="41"/>
     </row>
-    <row r="26" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B26" s="41" t="s">
         <v>17</v>
       </c>
@@ -3974,15 +3974,15 @@
       </c>
       <c r="E26" s="41"/>
     </row>
-    <row r="27" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="28" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="2:5" s="40" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="38"/>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
       <c r="E28" s="39"/>
     </row>
-    <row r="29" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="30" spans="2:5" s="33" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="30" spans="2:5" s="33" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B30" s="50" t="s">
         <v>19</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="31" spans="2:5" s="33" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:5" s="33" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B31" s="50" t="s">
         <v>21</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="32" spans="2:5" s="33" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:5" s="33" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B32" s="50" t="s">
         <v>23</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="33" spans="2:5" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:5" s="10" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B33" s="51" t="s">
         <v>25</v>
       </c>
@@ -4016,7 +4016,7 @@
       </c>
       <c r="E33" s="52"/>
     </row>
-    <row r="34" spans="2:5" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:5" s="10" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B34" s="51" t="s">
         <v>27</v>
       </c>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="E34" s="52"/>
     </row>
-    <row r="35" spans="2:5" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:5" s="10" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B35" s="51" t="s">
         <v>29</v>
       </c>
@@ -4036,15 +4036,15 @@
       </c>
       <c r="E35" s="52"/>
     </row>
-    <row r="36" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="37" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="37" spans="2:5" s="40" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="38"/>
       <c r="C37" s="38"/>
       <c r="D37" s="38"/>
       <c r="E37" s="39"/>
     </row>
-    <row r="38" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="39" spans="2:5" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="39" spans="2:5" s="10" customFormat="1" ht="30.45" x14ac:dyDescent="0.4">
       <c r="B39" s="51" t="s">
         <v>31</v>
       </c>
@@ -4054,7 +4054,7 @@
       </c>
       <c r="E39" s="53"/>
     </row>
-    <row r="40" spans="2:5" s="10" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:5" s="10" customFormat="1" ht="45.45" x14ac:dyDescent="0.4">
       <c r="B40" s="54" t="s">
         <v>32</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="41" spans="2:5" s="33" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:5" s="33" customFormat="1" ht="30.45" x14ac:dyDescent="0.4">
       <c r="B41" s="54" t="s">
         <v>33</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="2:5" s="10" customFormat="1" ht="30.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:5" s="10" customFormat="1" ht="30.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B42" s="50" t="s">
         <v>34</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="43" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B43" s="54" t="s">
         <v>35</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B44" s="54" t="s">
         <v>37</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="2:5" s="10" customFormat="1" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:5" s="10" customFormat="1" ht="16.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B45" s="54" t="s">
         <v>39</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="46" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B46" s="51" t="s">
         <v>40</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="2:5" s="10" customFormat="1" ht="45.7" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:5" s="10" customFormat="1" ht="45.9" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B47" s="55" t="s">
         <v>42</v>
       </c>
@@ -4124,17 +4124,17 @@
         <v>367</v>
       </c>
     </row>
-    <row r="48" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="49" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="49" spans="2:5" s="40" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="38"/>
       <c r="C49" s="38"/>
       <c r="D49" s="38"/>
       <c r="E49" s="39"/>
     </row>
-    <row r="50" spans="2:5" s="33" customFormat="1" ht="15.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:5" s="33" customFormat="1" ht="15.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B50" s="51"/>
     </row>
-    <row r="51" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:5" s="10" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B51" s="51" t="s">
         <v>43</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="2:5" s="10" customFormat="1" ht="15.7" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:5" s="10" customFormat="1" ht="15.9" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B52" s="51" t="s">
         <v>45</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>45848.59375</v>
       </c>
     </row>
-    <row r="53" spans="2:5" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:5" s="10" customFormat="1" ht="30.45" x14ac:dyDescent="0.4">
       <c r="B53" s="51" t="s">
         <v>46</v>
       </c>
@@ -4159,19 +4159,19 @@
         <v>368</v>
       </c>
     </row>
-    <row r="54" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B54" s="52"/>
       <c r="C54" s="52"/>
       <c r="D54" s="52"/>
     </row>
-    <row r="55" spans="2:5" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:5" s="40" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" s="38"/>
       <c r="C55" s="38"/>
       <c r="D55" s="38"/>
       <c r="E55" s="39"/>
     </row>
-    <row r="56" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="57" spans="2:5" s="10" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:5" s="33" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="57" spans="2:5" s="10" customFormat="1" ht="45.45" x14ac:dyDescent="0.4">
       <c r="B57" s="54" t="s">
         <v>47</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B58" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B52) &lt;= 60,
@@ -4198,7 +4198,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="59" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B59" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B53) &lt;= 60,
@@ -4216,7 +4216,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="60" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B60" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B54) &lt;= 60,
@@ -4234,7 +4234,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="61" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B61" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B55) &lt;= 60,
@@ -4252,7 +4252,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="62" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B62" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B56) &lt;= 60,
@@ -4270,7 +4270,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="63" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B63" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B57) &lt;= 60,
@@ -4288,7 +4288,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="64" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:5" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B64" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B58) &lt;= 60,
@@ -4306,7 +4306,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="65" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B65" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B59) &lt;= 60,
@@ -4324,7 +4324,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="66" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B66" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B60) &lt;= 60,
@@ -4342,7 +4342,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="67" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B67" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B61) &lt;= 60,
@@ -4360,7 +4360,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="68" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B68" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B62) &lt;= 60,
@@ -4378,7 +4378,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="69" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B69" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B63) &lt;= 60,
@@ -4396,7 +4396,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="70" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B70" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B64) &lt;= 60,
@@ -4414,7 +4414,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="71" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="71" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B71" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B65) &lt;= 60,
@@ -4432,7 +4432,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="72" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B72" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B66) &lt;= 60,
@@ -4450,7 +4450,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="73" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B73" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B67) &lt;= 60,
@@ -4468,7 +4468,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="74" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B74" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B68) &lt;= 60,
@@ -4486,7 +4486,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="75" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B75" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B69) &lt;= 60,
@@ -4504,7 +4504,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="76" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="76" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B76" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B70) &lt;= 60,
@@ -4522,7 +4522,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="77" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="77" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B77" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B71) &lt;= 60,
@@ -4540,7 +4540,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="78" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="78" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B78" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B72) &lt;= 60,
@@ -4558,7 +4558,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="79" spans="2:7" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="2:7" s="10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B79" s="54" t="s">
         <v>49</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.5">
+    <row r="80" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="B80" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B76) &lt;= 60,
@@ -4587,7 +4587,7 @@
       </c>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="B81" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B77) &lt;= 60,
@@ -4607,7 +4607,7 @@
       </c>
       <c r="G81"/>
     </row>
-    <row r="82" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="B82" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B78) &lt;= 60,
@@ -4627,7 +4627,7 @@
       </c>
       <c r="G82"/>
     </row>
-    <row r="83" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="83" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B83" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B79) &lt;= 60,
@@ -4646,7 +4646,7 @@
       </c>
       <c r="G83"/>
     </row>
-    <row r="84" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="84" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B84" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B80) &lt;= 60,
@@ -4665,7 +4665,7 @@
       </c>
       <c r="G84"/>
     </row>
-    <row r="85" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="85" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B85" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B81) &lt;= 60,
@@ -4684,7 +4684,7 @@
       </c>
       <c r="G85"/>
     </row>
-    <row r="86" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="86" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B86" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B82) &lt;= 60,
@@ -4703,7 +4703,7 @@
       </c>
       <c r="G86"/>
     </row>
-    <row r="87" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="87" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B87" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B83) &lt;= 60,
@@ -4722,7 +4722,7 @@
       </c>
       <c r="G87"/>
     </row>
-    <row r="88" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.5">
+    <row r="88" spans="2:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="B88" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B84) &lt;= 60,
@@ -4742,7 +4742,7 @@
       </c>
       <c r="G88"/>
     </row>
-    <row r="89" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="89" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B89" s="56" t="str">
         <f>IF(
   LEN(_carb_only!B85) &lt;= 60,
@@ -4761,7 +4761,7 @@
       </c>
       <c r="G89"/>
     </row>
-    <row r="90" spans="2:7" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="90" spans="2:7" s="10" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B90" s="54" t="s">
         <v>50</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="91" spans="2:7" s="10" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
+    <row r="91" spans="2:7" s="10" customFormat="1" ht="45.45" x14ac:dyDescent="0.4">
       <c r="B91" s="54" t="s">
         <v>51</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="92" spans="2:7" s="10" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
+    <row r="92" spans="2:7" s="10" customFormat="1" ht="45.45" x14ac:dyDescent="0.4">
       <c r="B92" s="54" t="s">
         <v>52</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="93" spans="2:7" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="93" spans="2:7" s="10" customFormat="1" ht="30.45" x14ac:dyDescent="0.4">
       <c r="B93" s="54" t="s">
         <v>53</v>
       </c>
@@ -4793,13 +4793,13 @@
         <v>373</v>
       </c>
     </row>
-    <row r="94" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="94" spans="2:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B94" s="52"/>
       <c r="D94" s="58"/>
     </row>
-    <row r="95" spans="2:7" s="17" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="96" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="97" spans="2:4" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="95" spans="2:7" s="17" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="96" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="97" spans="2:4" s="10" customFormat="1" ht="30.45" x14ac:dyDescent="0.4">
       <c r="B97" s="54" t="s">
         <v>54</v>
       </c>
@@ -4855,19 +4855,19 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="3" width="10.703125" customWidth="1"/>
-    <col min="4" max="4" width="80.703125" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
+    <col min="2" max="3" width="10.69140625" customWidth="1"/>
+    <col min="4" max="4" width="80.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -4891,17 +4891,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B9" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B10" s="6"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>61</v>
       </c>
@@ -4912,7 +4912,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B12" s="13" t="s">
         <v>64</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B13" s="13" t="s">
         <v>66</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B14" s="13" t="s">
         <v>68</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B15" s="13" t="s">
         <v>70</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B16" s="13" t="s">
         <v>72</v>
       </c>
@@ -4965,52 +4965,52 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -5032,31 +5032,31 @@
   <sheetViews>
     <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="45.703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.29296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="45.703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.69140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.61328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.69140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45.69140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
         <v>74</v>
       </c>
       <c r="F2" s="16"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="G3" s="2"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -5064,15 +5064,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B7" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>77</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B10" s="13" t="s">
         <v>79</v>
       </c>
@@ -5091,7 +5091,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:11" s="10" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B11" s="13" t="s">
         <v>81</v>
       </c>
@@ -5102,7 +5102,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="12" spans="1:11" s="10" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B12" s="13" t="s">
         <v>83</v>
       </c>
@@ -5113,7 +5113,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B13" s="13" t="s">
         <v>85</v>
       </c>
@@ -5124,15 +5124,15 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B14" s="10"/>
       <c r="C14" s="13"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B15" s="10"/>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B16" s="6" t="s">
         <v>87</v>
       </c>
@@ -5142,14 +5142,14 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.4">
       <c r="G17" s="2"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>88</v>
       </c>
@@ -5173,7 +5173,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="2:11" s="10" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:11" s="10" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B19" s="10">
         <v>1</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="2:11" s="10" customFormat="1" ht="86" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:11" s="10" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="B20" s="10">
         <v>2</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="2:11" s="10" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:11" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B21" s="10">
         <v>3</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="2:11" s="10" customFormat="1" ht="271.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:11" s="10" customFormat="1" ht="271.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="10">
         <v>4</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="2:11" s="10" customFormat="1" ht="157.69999999999999" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:11" s="10" customFormat="1" ht="174.9" x14ac:dyDescent="0.4">
       <c r="B23" s="10">
         <v>5</v>
       </c>
@@ -5271,7 +5271,7 @@
       </c>
       <c r="G23" s="13"/>
     </row>
-    <row r="24" spans="2:11" s="10" customFormat="1" ht="198.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:11" s="10" customFormat="1" ht="198.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="10">
         <v>6</v>
       </c>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="2:11" s="10" customFormat="1" ht="114.7" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:11" s="10" customFormat="1" ht="116.6" x14ac:dyDescent="0.4">
       <c r="B25" s="10">
         <v>7</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="2:11" s="10" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:11" s="10" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="10">
         <v>8</v>
       </c>
@@ -5327,7 +5327,7 @@
       </c>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="2:11" s="10" customFormat="1" ht="301" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:11" s="10" customFormat="1" ht="306" x14ac:dyDescent="0.4">
       <c r="B27" s="10">
         <v>9</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="2:11" s="10" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:11" s="10" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="B28" s="10">
         <v>10</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="2:11" s="10" customFormat="1" ht="100.35" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:11" s="10" customFormat="1" ht="131.15" x14ac:dyDescent="0.4">
       <c r="B29" s="10">
         <v>11</v>
       </c>
@@ -5382,7 +5382,7 @@
       </c>
       <c r="G29" s="13"/>
     </row>
-    <row r="30" spans="2:11" s="10" customFormat="1" ht="86" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:11" s="10" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
       <c r="B30" s="10">
         <v>12</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="2:11" s="10" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:11" s="10" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="B31" s="10">
         <v>13</v>
       </c>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="G31" s="13"/>
     </row>
-    <row r="32" spans="2:11" s="10" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:11" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B32" s="10">
         <v>14</v>
       </c>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="G32" s="13"/>
     </row>
-    <row r="33" spans="2:7" s="10" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:7" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B33" s="10">
         <v>15</v>
       </c>
@@ -5453,7 +5453,7 @@
       </c>
       <c r="G33" s="13"/>
     </row>
-    <row r="34" spans="2:7" s="10" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:7" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B34" s="10">
         <v>16</v>
       </c>
@@ -5471,7 +5471,7 @@
       </c>
       <c r="G34" s="13"/>
     </row>
-    <row r="35" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B35" s="10">
         <v>17</v>
       </c>
@@ -5480,7 +5480,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
     </row>
-    <row r="36" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B36" s="10">
         <v>18</v>
       </c>
@@ -5489,7 +5489,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
     </row>
-    <row r="37" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B37" s="10">
         <v>19</v>
       </c>
@@ -5498,7 +5498,7 @@
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
     </row>
-    <row r="38" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B38" s="10">
         <v>20</v>
       </c>
@@ -5507,7 +5507,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
     </row>
-    <row r="39" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B39" s="10">
         <v>21</v>
       </c>
@@ -5516,7 +5516,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
     </row>
-    <row r="40" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B40" s="10">
         <v>22</v>
       </c>
@@ -5525,7 +5525,7 @@
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
     </row>
-    <row r="41" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B41" s="10">
         <v>23</v>
       </c>
@@ -5534,7 +5534,7 @@
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
     </row>
-    <row r="42" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B42" s="10">
         <v>24</v>
       </c>
@@ -5543,7 +5543,7 @@
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
     </row>
-    <row r="43" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B43" s="10">
         <v>25</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
     </row>
-    <row r="44" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B44" s="10">
         <v>26</v>
       </c>
@@ -5561,7 +5561,7 @@
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
     </row>
-    <row r="45" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B45" s="10">
         <v>27</v>
       </c>
@@ -5570,7 +5570,7 @@
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
     </row>
-    <row r="46" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B46" s="10">
         <v>28</v>
       </c>
@@ -5579,7 +5579,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
     </row>
-    <row r="47" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B47" s="10">
         <v>29</v>
       </c>
@@ -5588,7 +5588,7 @@
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
     </row>
-    <row r="48" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B48" s="10">
         <v>30</v>
       </c>
@@ -5597,7 +5597,7 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B49" s="10">
         <v>31</v>
       </c>
@@ -5606,7 +5606,7 @@
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
     </row>
-    <row r="50" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B50" s="10">
         <v>32</v>
       </c>
@@ -5615,7 +5615,7 @@
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
     </row>
-    <row r="51" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B51" s="10">
         <v>33</v>
       </c>
@@ -5624,7 +5624,7 @@
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
     </row>
-    <row r="52" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B52" s="10">
         <v>34</v>
       </c>
@@ -5633,7 +5633,7 @@
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
     </row>
-    <row r="53" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B53" s="10">
         <v>35</v>
       </c>
@@ -5642,7 +5642,7 @@
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
     </row>
-    <row r="54" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B54" s="10">
         <v>36</v>
       </c>
@@ -5651,7 +5651,7 @@
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
     </row>
-    <row r="55" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B55" s="10">
         <v>37</v>
       </c>
@@ -5660,7 +5660,7 @@
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
     </row>
-    <row r="56" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B56" s="10">
         <v>38</v>
       </c>
@@ -5669,7 +5669,7 @@
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
     </row>
-    <row r="57" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B57" s="10">
         <v>39</v>
       </c>
@@ -5678,7 +5678,7 @@
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
     </row>
-    <row r="58" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B58" s="10">
         <v>40</v>
       </c>
@@ -5687,7 +5687,7 @@
       <c r="F58" s="13"/>
       <c r="G58" s="13"/>
     </row>
-    <row r="59" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B59" s="10">
         <v>41</v>
       </c>
@@ -5696,7 +5696,7 @@
       <c r="F59" s="13"/>
       <c r="G59" s="13"/>
     </row>
-    <row r="60" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B60" s="10">
         <v>42</v>
       </c>
@@ -5705,7 +5705,7 @@
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
     </row>
-    <row r="61" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B61" s="10">
         <v>43</v>
       </c>
@@ -5714,7 +5714,7 @@
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
     </row>
-    <row r="62" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B62" s="10">
         <v>44</v>
       </c>
@@ -5723,7 +5723,7 @@
       <c r="F62" s="13"/>
       <c r="G62" s="13"/>
     </row>
-    <row r="63" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B63" s="10">
         <v>45</v>
       </c>
@@ -5732,7 +5732,7 @@
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
     </row>
-    <row r="64" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B64" s="10">
         <v>46</v>
       </c>
@@ -5741,7 +5741,7 @@
       <c r="F64" s="13"/>
       <c r="G64" s="13"/>
     </row>
-    <row r="65" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B65" s="10">
         <v>47</v>
       </c>
@@ -5750,7 +5750,7 @@
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
     </row>
-    <row r="66" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B66" s="10">
         <v>48</v>
       </c>
@@ -5759,7 +5759,7 @@
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
     </row>
-    <row r="67" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B67" s="10">
         <v>49</v>
       </c>
@@ -5768,7 +5768,7 @@
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
     </row>
-    <row r="68" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B68" s="10">
         <v>50</v>
       </c>
@@ -5777,7 +5777,7 @@
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
     </row>
-    <row r="69" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B69" s="10">
         <v>51</v>
       </c>
@@ -5786,7 +5786,7 @@
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
     </row>
-    <row r="70" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B70" s="10">
         <v>52</v>
       </c>
@@ -5795,7 +5795,7 @@
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
     </row>
-    <row r="71" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B71" s="10">
         <v>53</v>
       </c>
@@ -5804,7 +5804,7 @@
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
     </row>
-    <row r="72" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B72" s="10">
         <v>54</v>
       </c>
@@ -5813,7 +5813,7 @@
       <c r="F72" s="13"/>
       <c r="G72" s="13"/>
     </row>
-    <row r="73" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B73" s="10">
         <v>55</v>
       </c>
@@ -5822,7 +5822,7 @@
       <c r="F73" s="13"/>
       <c r="G73" s="13"/>
     </row>
-    <row r="74" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B74" s="10">
         <v>56</v>
       </c>
@@ -5831,7 +5831,7 @@
       <c r="F74" s="13"/>
       <c r="G74" s="13"/>
     </row>
-    <row r="75" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B75" s="10">
         <v>57</v>
       </c>
@@ -5840,7 +5840,7 @@
       <c r="F75" s="13"/>
       <c r="G75" s="13"/>
     </row>
-    <row r="76" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="76" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B76" s="10">
         <v>58</v>
       </c>
@@ -5849,7 +5849,7 @@
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
     </row>
-    <row r="77" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="77" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B77" s="10">
         <v>59</v>
       </c>
@@ -5858,7 +5858,7 @@
       <c r="F77" s="13"/>
       <c r="G77" s="13"/>
     </row>
-    <row r="78" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="78" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B78" s="10">
         <v>60</v>
       </c>
@@ -5867,7 +5867,7 @@
       <c r="F78" s="13"/>
       <c r="G78" s="13"/>
     </row>
-    <row r="79" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B79" s="10">
         <v>61</v>
       </c>
@@ -5876,7 +5876,7 @@
       <c r="F79" s="13"/>
       <c r="G79" s="13"/>
     </row>
-    <row r="80" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="80" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B80" s="10">
         <v>62</v>
       </c>
@@ -5885,7 +5885,7 @@
       <c r="F80" s="13"/>
       <c r="G80" s="13"/>
     </row>
-    <row r="81" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B81" s="10">
         <v>63</v>
       </c>
@@ -5894,7 +5894,7 @@
       <c r="F81" s="13"/>
       <c r="G81" s="13"/>
     </row>
-    <row r="82" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B82" s="10">
         <v>64</v>
       </c>
@@ -5903,7 +5903,7 @@
       <c r="F82" s="13"/>
       <c r="G82" s="13"/>
     </row>
-    <row r="83" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B83" s="10">
         <v>65</v>
       </c>
@@ -5912,7 +5912,7 @@
       <c r="F83" s="13"/>
       <c r="G83" s="13"/>
     </row>
-    <row r="84" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="84" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B84" s="10">
         <v>66</v>
       </c>
@@ -5922,7 +5922,7 @@
       <c r="F84" s="13"/>
       <c r="G84" s="23"/>
     </row>
-    <row r="85" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="85" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B85" s="10">
         <v>67</v>
       </c>
@@ -5931,7 +5931,7 @@
       <c r="F85" s="13"/>
       <c r="G85" s="13"/>
     </row>
-    <row r="86" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="86" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B86" s="10">
         <v>68</v>
       </c>
@@ -5940,7 +5940,7 @@
       <c r="F86" s="13"/>
       <c r="G86" s="13"/>
     </row>
-    <row r="87" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="87" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B87" s="10">
         <v>69</v>
       </c>
@@ -5949,7 +5949,7 @@
       <c r="F87" s="13"/>
       <c r="G87" s="13"/>
     </row>
-    <row r="88" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="88" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B88" s="10">
         <v>70</v>
       </c>
@@ -5958,7 +5958,7 @@
       <c r="F88" s="13"/>
       <c r="G88" s="19"/>
     </row>
-    <row r="89" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="89" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B89" s="10">
         <v>71</v>
       </c>
@@ -5967,7 +5967,7 @@
       <c r="F89" s="13"/>
       <c r="G89" s="19"/>
     </row>
-    <row r="90" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="90" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B90" s="10">
         <v>72</v>
       </c>
@@ -5976,7 +5976,7 @@
       <c r="F90" s="13"/>
       <c r="G90" s="13"/>
     </row>
-    <row r="91" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="91" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B91" s="10">
         <v>73</v>
       </c>
@@ -5985,7 +5985,7 @@
       <c r="F91" s="13"/>
       <c r="G91" s="19"/>
     </row>
-    <row r="92" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="92" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B92" s="10">
         <v>74</v>
       </c>
@@ -5994,7 +5994,7 @@
       <c r="F92" s="13"/>
       <c r="G92" s="13"/>
     </row>
-    <row r="93" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="93" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B93" s="10">
         <v>75</v>
       </c>
@@ -6003,7 +6003,7 @@
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
     </row>
-    <row r="94" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="94" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B94" s="10">
         <v>76</v>
       </c>
@@ -6012,7 +6012,7 @@
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
     </row>
-    <row r="95" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B95" s="10">
         <v>77</v>
       </c>
@@ -6021,7 +6021,7 @@
       <c r="F95" s="13"/>
       <c r="G95" s="13"/>
     </row>
-    <row r="96" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="96" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B96" s="10">
         <v>78</v>
       </c>
@@ -6030,7 +6030,7 @@
       <c r="F96" s="13"/>
       <c r="G96" s="13"/>
     </row>
-    <row r="97" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="97" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B97" s="10">
         <v>79</v>
       </c>
@@ -6039,7 +6039,7 @@
       <c r="F97" s="13"/>
       <c r="G97" s="13"/>
     </row>
-    <row r="98" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="98" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B98" s="10">
         <v>80</v>
       </c>
@@ -6048,7 +6048,7 @@
       <c r="F98" s="13"/>
       <c r="G98" s="13"/>
     </row>
-    <row r="99" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="99" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B99" s="10">
         <v>81</v>
       </c>
@@ -6057,7 +6057,7 @@
       <c r="F99" s="13"/>
       <c r="G99" s="13"/>
     </row>
-    <row r="100" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="100" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B100" s="10">
         <v>82</v>
       </c>
@@ -6066,7 +6066,7 @@
       <c r="F100" s="13"/>
       <c r="G100" s="13"/>
     </row>
-    <row r="101" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="101" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B101" s="10">
         <v>83</v>
       </c>
@@ -6075,7 +6075,7 @@
       <c r="F101" s="13"/>
       <c r="G101" s="13"/>
     </row>
-    <row r="102" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="102" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B102" s="10">
         <v>84</v>
       </c>
@@ -6084,7 +6084,7 @@
       <c r="F102" s="13"/>
       <c r="G102" s="13"/>
     </row>
-    <row r="103" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="103" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B103" s="10">
         <v>85</v>
       </c>
@@ -6093,7 +6093,7 @@
       <c r="F103" s="13"/>
       <c r="G103" s="13"/>
     </row>
-    <row r="104" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="104" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B104" s="10">
         <v>86</v>
       </c>
@@ -6102,7 +6102,7 @@
       <c r="F104" s="13"/>
       <c r="G104" s="13"/>
     </row>
-    <row r="105" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="105" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B105" s="10">
         <v>87</v>
       </c>
@@ -6112,7 +6112,7 @@
       <c r="F105" s="13"/>
       <c r="G105" s="13"/>
     </row>
-    <row r="106" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="106" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B106" s="10">
         <v>88</v>
       </c>
@@ -6122,7 +6122,7 @@
       <c r="F106" s="13"/>
       <c r="G106" s="13"/>
     </row>
-    <row r="107" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="107" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B107" s="10">
         <v>89</v>
       </c>
@@ -6132,7 +6132,7 @@
       <c r="F107" s="13"/>
       <c r="G107" s="13"/>
     </row>
-    <row r="108" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="108" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B108" s="10">
         <v>90</v>
       </c>
@@ -6142,7 +6142,7 @@
       <c r="F108" s="13"/>
       <c r="G108" s="13"/>
     </row>
-    <row r="109" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="109" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B109" s="10">
         <v>91</v>
       </c>
@@ -6152,7 +6152,7 @@
       <c r="F109" s="13"/>
       <c r="G109" s="13"/>
     </row>
-    <row r="110" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="110" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B110" s="10">
         <v>92</v>
       </c>
@@ -6162,7 +6162,7 @@
       <c r="F110" s="13"/>
       <c r="G110" s="13"/>
     </row>
-    <row r="111" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="111" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B111" s="10">
         <v>93</v>
       </c>
@@ -6171,7 +6171,7 @@
       <c r="F111" s="13"/>
       <c r="G111" s="13"/>
     </row>
-    <row r="112" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="112" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B112" s="10">
         <v>94</v>
       </c>
@@ -6181,7 +6181,7 @@
       <c r="F112" s="13"/>
       <c r="G112" s="13"/>
     </row>
-    <row r="113" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="113" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B113" s="10">
         <v>95</v>
       </c>
@@ -6191,7 +6191,7 @@
       <c r="F113" s="13"/>
       <c r="G113" s="13"/>
     </row>
-    <row r="114" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="114" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B114" s="10">
         <v>96</v>
       </c>
@@ -6201,7 +6201,7 @@
       <c r="F114" s="13"/>
       <c r="G114" s="13"/>
     </row>
-    <row r="115" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="115" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B115" s="10">
         <v>97</v>
       </c>
@@ -6211,7 +6211,7 @@
       <c r="F115" s="13"/>
       <c r="G115" s="13"/>
     </row>
-    <row r="116" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="116" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B116" s="10">
         <v>98</v>
       </c>
@@ -6221,7 +6221,7 @@
       <c r="F116" s="13"/>
       <c r="G116" s="13"/>
     </row>
-    <row r="117" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="117" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B117" s="10">
         <v>99</v>
       </c>
@@ -6231,7 +6231,7 @@
       <c r="F117" s="13"/>
       <c r="G117" s="13"/>
     </row>
-    <row r="118" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="118" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B118" s="10">
         <v>100</v>
       </c>
@@ -6274,22 +6274,22 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="2" width="92.29296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.1171875" customWidth="1"/>
-    <col min="4" max="5" width="16.703125" customWidth="1"/>
-    <col min="6" max="17" width="16.703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
+    <col min="2" max="2" width="92.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.07421875" customWidth="1"/>
+    <col min="4" max="5" width="16.69140625" customWidth="1"/>
+    <col min="6" max="17" width="16.69140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
         <v>121</v>
       </c>
       <c r="F2" s="16"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -6309,7 +6309,7 @@
       <c r="P4"/>
       <c r="Q4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -6328,7 +6328,7 @@
       <c r="P5"/>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -6347,7 +6347,7 @@
       <c r="P6"/>
       <c r="Q6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -6360,156 +6360,156 @@
       <c r="P7"/>
       <c r="Q7"/>
     </row>
-    <row r="10" spans="1:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:17" s="21" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="21" t="s">
         <v>125</v>
       </c>
       <c r="D10"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B12" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B20" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B35" s="6" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B45" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
         <v>44</v>
       </c>
@@ -6524,7 +6524,7 @@
       <c r="P47"/>
       <c r="Q47"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
         <v>152</v>
       </c>
@@ -6538,15 +6538,15 @@
       <c r="P48"/>
       <c r="Q48"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B50" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B51" s="6"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
         <v>154</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
         <v>155</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
         <v>156</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
         <v>157</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
         <v>158</v>
       </c>
@@ -6606,7 +6606,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
         <v>159</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
         <v>160</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
         <v>161</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
         <v>162</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
         <v>163</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
         <v>164</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
         <v>165</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
         <v>166</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
         <v>167</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
         <v>168</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
         <v>169</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
         <v>170</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
         <v>171</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
         <v>172</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
         <v>173</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
         <v>174</v>
       </c>
@@ -6798,18 +6798,18 @@
         <v>174</v>
       </c>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B73" s="6"/>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B74" s="6" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B75" s="6"/>
     </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
         <v>176</v>
       </c>
@@ -6825,7 +6825,7 @@
       <c r="P76"/>
       <c r="Q76"/>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
         <v>177</v>
       </c>
@@ -6841,7 +6841,7 @@
       <c r="P77"/>
       <c r="Q77"/>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
         <v>178</v>
       </c>
@@ -6857,7 +6857,7 @@
       <c r="P78"/>
       <c r="Q78"/>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
         <v>179</v>
       </c>
@@ -6873,7 +6873,7 @@
       <c r="P79"/>
       <c r="Q79"/>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
         <v>180</v>
       </c>
@@ -6889,7 +6889,7 @@
       <c r="P80"/>
       <c r="Q80"/>
     </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
         <v>181</v>
       </c>
@@ -6905,7 +6905,7 @@
       <c r="P81"/>
       <c r="Q81"/>
     </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
         <v>182</v>
       </c>
@@ -6921,7 +6921,7 @@
       <c r="P82"/>
       <c r="Q82"/>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B83" t="s">
         <v>183</v>
       </c>
@@ -6937,7 +6937,7 @@
       <c r="P83"/>
       <c r="Q83"/>
     </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B84" t="s">
         <v>184</v>
       </c>
@@ -6953,7 +6953,7 @@
       <c r="P84"/>
       <c r="Q84"/>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B85" t="s">
         <v>185</v>
       </c>
@@ -6969,22 +6969,22 @@
       <c r="P85"/>
       <c r="Q85"/>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B86" s="6"/>
     </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.4">
       <c r="G87"/>
     </row>
-    <row r="88" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="88" spans="2:17" s="21" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B88" s="21" t="s">
         <v>186</v>
       </c>
       <c r="D88"/>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.4">
       <c r="G89"/>
     </row>
-    <row r="90" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="90" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B90" s="7" t="s">
         <v>187</v>
       </c>
@@ -6992,13 +6992,13 @@
       <c r="F90"/>
       <c r="Q90"/>
     </row>
-    <row r="91" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="91" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B91" s="6"/>
       <c r="E91" s="3"/>
       <c r="F91"/>
       <c r="Q91"/>
     </row>
-    <row r="92" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="92" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
         <v>36</v>
       </c>
@@ -7006,7 +7006,7 @@
       <c r="F92"/>
       <c r="Q92"/>
     </row>
-    <row r="93" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B93" t="str" cm="1">
         <f t="array" ref="B93:B97">_carb_only_table_01[]</f>
         <v>No leak detected</v>
@@ -7015,7 +7015,7 @@
       <c r="F93"/>
       <c r="Q93"/>
     </row>
-    <row r="94" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="94" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B94" t="str">
         <v>An intentional or allowable vent (i.e. the operator was aware of, and/or would not repair)</v>
       </c>
@@ -7023,7 +7023,7 @@
       <c r="F94"/>
       <c r="Q94"/>
     </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B95" t="str">
         <v>Due to a temporary activity (i.e. would be resolved without corrective action when the activity is completed)</v>
       </c>
@@ -7031,7 +7031,7 @@
       <c r="F95"/>
       <c r="Q95"/>
     </row>
-    <row r="96" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="96" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B96" t="str">
         <v>Operator was aware of the leak prior to receiving the CARB plume notification and/or repairs were in progress</v>
       </c>
@@ -7039,7 +7039,7 @@
       <c r="F96"/>
       <c r="Q96"/>
     </row>
-    <row r="97" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="97" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B97" t="str">
         <v>An unintentional leak (i.e. the operator was not aware of, and could be repaired if discovered)</v>
       </c>
@@ -7047,23 +7047,23 @@
       <c r="F97"/>
       <c r="Q97"/>
     </row>
-    <row r="98" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="98" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E98" s="3"/>
       <c r="F98"/>
       <c r="Q98"/>
     </row>
-    <row r="99" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="99" spans="2:17" s="21" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B99" s="21" t="s">
         <v>188</v>
       </c>
       <c r="D99"/>
     </row>
-    <row r="100" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="100" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E100" s="3"/>
       <c r="F100"/>
       <c r="Q100"/>
     </row>
-    <row r="101" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="101" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B101" s="7" t="s">
         <v>187</v>
       </c>
@@ -7071,90 +7071,90 @@
       <c r="F101"/>
       <c r="Q101"/>
     </row>
-    <row r="102" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="102" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B102" s="6"/>
       <c r="E102" s="3"/>
       <c r="F102"/>
       <c r="Q102"/>
     </row>
-    <row r="103" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="103" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B103" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="104" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="104" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B104" t="str" cm="1">
         <f t="array" ref="B104:B115">_carb_only_table_02[]</f>
         <v>Animal housing/barn/corral/lot</v>
       </c>
     </row>
-    <row r="105" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="105" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B105" t="str">
         <v>Biogas conditioning/upgrading equipment</v>
       </c>
     </row>
-    <row r="106" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="106" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B106" t="str">
         <v>Biogas moving/handling equipment</v>
       </c>
     </row>
-    <row r="107" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="107" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B107" t="str">
         <v>Digester component (other)</v>
       </c>
     </row>
-    <row r="108" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="108" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B108" t="str">
         <v>Digester cover</v>
       </c>
     </row>
-    <row r="109" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="109" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B109" t="str">
         <v>Effluent pond</v>
       </c>
     </row>
-    <row r="110" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="110" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B110" t="str">
         <v>Interconnection/pipeline</v>
       </c>
     </row>
-    <row r="111" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="111" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B111" t="str">
         <v>Manure collection pit</v>
       </c>
     </row>
-    <row r="112" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="112" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B112" t="str">
         <v>Manure separator</v>
       </c>
     </row>
-    <row r="113" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="113" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B113" t="str">
         <v>Open lagoon</v>
       </c>
     </row>
-    <row r="114" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="114" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B114" t="str">
         <v xml:space="preserve">Other </v>
       </c>
     </row>
-    <row r="115" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="115" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B115" t="str">
         <v>Stacking slab/stockpile/other manure storage</v>
       </c>
     </row>
-    <row r="118" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="118" spans="2:17" s="21" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B118" s="21" t="s">
         <v>189</v>
       </c>
       <c r="D118"/>
     </row>
-    <row r="119" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="119" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E119" s="3"/>
       <c r="F119"/>
       <c r="Q119"/>
     </row>
-    <row r="120" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="120" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B120" s="7" t="s">
         <v>187</v>
       </c>
@@ -7162,65 +7162,65 @@
       <c r="F120"/>
       <c r="Q120"/>
     </row>
-    <row r="121" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="121" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B121" s="6"/>
       <c r="E121" s="3"/>
       <c r="F121"/>
       <c r="Q121"/>
     </row>
-    <row r="122" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="122" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B122" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="123" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="123" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B123" t="str" cm="1">
         <f t="array" ref="B123:B129">_carb_only_table_03[]</f>
         <v>Construction activity</v>
       </c>
     </row>
-    <row r="124" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="124" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B124" t="str">
         <v>Damaged/broken component (e.g. tear in digester cover, loose flange/port/seal)</v>
       </c>
     </row>
-    <row r="125" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="125" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B125" t="str">
         <v>Maintenance/repair/testing activity</v>
       </c>
     </row>
-    <row r="126" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="126" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B126" t="str">
         <v>Manure management activity</v>
       </c>
     </row>
-    <row r="127" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="127" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B127" t="str">
         <v>Other</v>
       </c>
     </row>
-    <row r="128" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="128" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B128" t="str">
         <v>Venting-emergency/temporary</v>
       </c>
     </row>
-    <row r="129" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="129" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B129" t="str">
         <v>Venting-intentional/routine</v>
       </c>
     </row>
-    <row r="132" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="132" spans="2:17" s="21" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B132" s="21" t="s">
         <v>190</v>
       </c>
       <c r="D132"/>
     </row>
-    <row r="133" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="133" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E133" s="3"/>
       <c r="F133"/>
       <c r="Q133"/>
     </row>
-    <row r="134" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="134" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B134" s="7" t="s">
         <v>187</v>
       </c>
@@ -7228,40 +7228,40 @@
       <c r="F134"/>
       <c r="Q134"/>
     </row>
-    <row r="135" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="135" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B135" s="6"/>
       <c r="E135" s="3"/>
       <c r="F135"/>
       <c r="Q135"/>
     </row>
-    <row r="136" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="136" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B136" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="137" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="137" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B137" t="str" cm="1">
         <f t="array" ref="B137:B138">_carb_only_table_04[]</f>
         <v>Yes</v>
       </c>
     </row>
-    <row r="138" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="138" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B138" t="str">
         <v>No</v>
       </c>
     </row>
-    <row r="141" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="141" spans="2:17" s="21" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B141" s="21" t="s">
         <v>191</v>
       </c>
       <c r="D141"/>
     </row>
-    <row r="142" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="142" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E142" s="3"/>
       <c r="F142"/>
       <c r="Q142"/>
     </row>
-    <row r="143" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="143" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B143" s="7" t="s">
         <v>187</v>
       </c>
@@ -7269,18 +7269,18 @@
       <c r="F143"/>
       <c r="Q143"/>
     </row>
-    <row r="144" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="144" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B144" s="6"/>
       <c r="E144" s="3"/>
       <c r="F144"/>
       <c r="Q144"/>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B145" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B146" t="str" cm="1">
         <f t="array" ref="B146:C166">_carb_only_table_05[]</f>
         <v>Solid/dry scrape manure collection</v>
@@ -7289,7 +7289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B147" t="str">
         <v>Vacuum manure collection</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B148" t="str">
         <v>Liquid/flush manure collection</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B149" t="str">
         <v>Pasture</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B150" t="str">
         <v>Dry lot/corral</v>
       </c>
@@ -7321,7 +7321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B151" t="str">
         <v>Solid storage</v>
       </c>
@@ -7329,7 +7329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B152" t="str">
         <v>Solar drying</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B153" t="str">
         <v>Composting (aerated, in vessel, windrows)</v>
       </c>
@@ -7345,7 +7345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B154" t="str">
         <v>Compost bedded pack barn</v>
       </c>
@@ -7353,7 +7353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B155" t="str">
         <v>Slatted floor pit storage</v>
       </c>
@@ -7361,7 +7361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B156" t="str">
         <v>Anaerobic Lagoon</v>
       </c>
@@ -7369,7 +7369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B157" t="str">
         <v>Anaerobic digester</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B158" t="str">
         <v>Vermifiltration</v>
       </c>
@@ -7385,7 +7385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B159" t="str">
         <v>Liquid/slurry</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B160" t="str">
         <v>Mechanical separator (screens, centrifuge, press)</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B161" t="str">
         <v>Gravity-based separator (settling basin, sand lane)</v>
       </c>
@@ -7409,7 +7409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B162" t="str">
         <v>Weeping wall</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B163" t="str">
         <v>Flocculation</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B164" t="str">
         <v>Daily spread</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B165" t="str">
         <v>Land application (flood)</v>
       </c>
@@ -7441,7 +7441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B166" t="str">
         <v>Land application (subsurface drip)</v>
       </c>
@@ -7449,18 +7449,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="2:17" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="180" spans="2:17" s="21" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B180" s="21" t="s">
         <v>192</v>
       </c>
       <c r="D180"/>
     </row>
-    <row r="181" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="181" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E181" s="3"/>
       <c r="F181"/>
       <c r="Q181"/>
     </row>
-    <row r="182" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="182" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B182" s="7" t="s">
         <v>187</v>
       </c>
@@ -7468,18 +7468,18 @@
       <c r="F182"/>
       <c r="Q182"/>
     </row>
-    <row r="183" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="183" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B183" s="6"/>
       <c r="E183" s="3"/>
       <c r="F183"/>
       <c r="Q183"/>
     </row>
-    <row r="184" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="184" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B184" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="185" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="185" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B185" t="str" cm="1">
         <f t="array" ref="B185:C194">_carb_only_table_06[]</f>
         <v>Biogas conditioning (e.g., hydrogen sulfide, moisture, particulate removal)</v>
@@ -7488,7 +7488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="186" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B186" t="str">
         <v>Biogas moving and handling equipement (e.g., blower, compressor, low pressure gas pipelines)</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="187" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B187" t="str">
         <v>Biomethane upgrading (e.g., membrane or other form of CO2 removal)</v>
       </c>
@@ -7504,7 +7504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="188" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B188" t="str">
         <v>Covered lagoon anaerobic digester</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="189" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B189" t="str">
         <v>In-vessel anaerobic digester</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="190" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B190" t="str">
         <v>Electricity generation or other combustion equipment</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="191" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B191" t="str">
         <v>Heating/process fuel equipment</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="192" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B192" t="str">
         <v>Fuel cells</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B193" t="str">
         <v>Common carrier gas pipeline (Interconnection point of receipt)</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B194" t="str">
         <v>Onsite fuel use or dispensing</v>
       </c>
@@ -7587,20 +7587,20 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="3" width="30.703125" customWidth="1"/>
-    <col min="4" max="9" width="8.703125" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
+    <col min="2" max="3" width="30.69140625" customWidth="1"/>
+    <col min="4" max="9" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
         <v>193</v>
       </c>
       <c r="F2" s="16"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -7616,7 +7616,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="11" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:6" s="11" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="11" t="s">
         <v>198</v>
       </c>
@@ -7641,7 +7641,7 @@
       </c>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>200</v>
       </c>
@@ -7664,19 +7664,19 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="3" width="30.703125" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
+    <col min="2" max="3" width="30.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
         <v>193</v>
       </c>
       <c r="F2" s="16"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -7684,7 +7684,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -7692,7 +7692,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -7708,12 +7708,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:6" s="11" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:6" s="11" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="11" t="s">
         <v>205</v>
       </c>
@@ -7722,7 +7722,7 @@
       </c>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>207</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>209</v>
       </c>
@@ -7754,23 +7754,23 @@
       <selection activeCell="A11" sqref="A11:F71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="2" width="25.1171875" customWidth="1"/>
-    <col min="3" max="3" width="16.29296875" customWidth="1"/>
-    <col min="4" max="4" width="51.87890625" customWidth="1"/>
-    <col min="5" max="5" width="16.29296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
+    <col min="2" max="2" width="25.07421875" customWidth="1"/>
+    <col min="3" max="3" width="16.3046875" customWidth="1"/>
+    <col min="4" max="4" width="51.84375" customWidth="1"/>
+    <col min="5" max="5" width="16.3046875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="99" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
         <v>211</v>
       </c>
       <c r="F2" s="16"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -7780,26 +7780,26 @@
       <c r="C4" s="1"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C5" s="1"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C6" s="1"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C7" s="1"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C8" s="1"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:6" s="11" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="11" t="s">
         <v>198</v>
       </c>
@@ -7816,7 +7816,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>200</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>200</v>
       </c>
@@ -7847,7 +7847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>200</v>
       </c>
@@ -7861,7 +7861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>200</v>
       </c>
@@ -7875,7 +7875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>200</v>
       </c>
@@ -7889,7 +7889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>200</v>
       </c>
@@ -7903,7 +7903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>200</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>200</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>200</v>
       </c>
@@ -7945,7 +7945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>200</v>
       </c>
@@ -7959,7 +7959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>200</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>200</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>200</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>200</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>200</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>200</v>
       </c>
@@ -8046,7 +8046,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>200</v>
       </c>
@@ -8063,7 +8063,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>200</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>200</v>
       </c>
@@ -8097,7 +8097,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>200</v>
       </c>
@@ -8114,7 +8114,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>200</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>200</v>
       </c>
@@ -8145,7 +8145,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>200</v>
       </c>
@@ -8159,7 +8159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>200</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>200</v>
       </c>
@@ -8193,7 +8193,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>200</v>
       </c>
@@ -8210,7 +8210,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>200</v>
       </c>
@@ -8227,7 +8227,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>200</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>7143</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>200</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>200</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>200</v>
       </c>
@@ -8286,7 +8286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>200</v>
       </c>
@@ -8303,7 +8303,7 @@
         <v>36.076599999999999</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>200</v>
       </c>
@@ -8320,7 +8320,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>200</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>-119.44289999999999</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>200</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>200</v>
       </c>
@@ -8365,7 +8365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
         <v>200</v>
       </c>
@@ -8379,7 +8379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
         <v>200</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
         <v>200</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
         <v>200</v>
       </c>
@@ -8421,7 +8421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
         <v>200</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
         <v>200</v>
       </c>
@@ -8449,7 +8449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
         <v>200</v>
       </c>
@@ -8463,7 +8463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
         <v>200</v>
       </c>
@@ -8477,7 +8477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
         <v>200</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
         <v>200</v>
       </c>
@@ -8505,7 +8505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
         <v>200</v>
       </c>
@@ -8519,7 +8519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
         <v>200</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
         <v>200</v>
       </c>
@@ -8547,7 +8547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
         <v>200</v>
       </c>
@@ -8561,7 +8561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
         <v>200</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
         <v>200</v>
       </c>
@@ -8589,7 +8589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
         <v>200</v>
       </c>
@@ -8603,7 +8603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
         <v>200</v>
       </c>
@@ -8617,7 +8617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
         <v>200</v>
       </c>
@@ -8631,7 +8631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
         <v>200</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
         <v>200</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
         <v>200</v>
       </c>
@@ -8676,7 +8676,7 @@
         <v>45782.517916666664</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
         <v>200</v>
       </c>
@@ -8690,7 +8690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
         <v>200</v>
       </c>
@@ -8704,7 +8704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
         <v>200</v>
       </c>
@@ -8730,6 +8730,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E9A34E7C7C736409D4BDE6375CCC276" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cf521a6d855790dbe6a6d894ff439cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32" xmlns:ns3="e20ceb87-0d79-402a-b4b9-75d78589c76d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45aa6d812898c4b0f52b4c3685679ce" ns2:_="" ns3:_="">
     <xsd:import namespace="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
@@ -8964,27 +8984,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
+    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC83B422-5B73-4269-9006-1DDE9C149499}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9003,25 +9022,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
-    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{9de5aaee-7788-40b1-a438-c0ccc98c87cc}" enabled="0" method="" siteId="{9de5aaee-7788-40b1-a438-c0ccc98c87cc}" removed="1"/>

</xml_diff>

<commit_message>
updating base and upload routes to avoid double flash messaging
</commit_message>
<xml_diff>
--- a/feedback_forms/testing_versions/standard/dairy_digester_operator_feedback_v006_test_01_good_data.xlsx
+++ b/feedback_forms/testing_versions/standard/dairy_digester_operator_feedback_v006_test_01_good_data.xlsx
@@ -8,19 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\local\cursor\feedback_portal\feedback_forms\testing_versions\standard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655750F0-5FFB-4AC5-9462-886722AB6D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ZZdeBZIs3h22LxegpdwwuHpsWEWuB9x+vvy4q5aW62Xkr4aTJmE005hpcsO5kgTp7rwoerT5PSsZglAASxcSXg==" workbookSaltValue="WgC7rnmlwtCTlwVo9LJMCQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEB7313-BDF7-4FAA-B08A-3600741061CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="4491" windowWidth="21729" windowHeight="13260" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="8786" yWindow="2391" windowWidth="21728" windowHeight="13260" tabRatio="705" activeTab="4" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
-    <sheet name="_versioning" sheetId="9" state="veryHidden" r:id="rId2"/>
-    <sheet name="_issue_tracking" sheetId="7" state="veryHidden" r:id="rId3"/>
-    <sheet name="_carb_only" sheetId="2" state="veryHidden" r:id="rId4"/>
-    <sheet name="_json_schema" sheetId="3" state="veryHidden" r:id="rId5"/>
-    <sheet name="_json_metadata" sheetId="4" state="veryHidden" r:id="rId6"/>
-    <sheet name="_named_ranges" sheetId="8" state="veryHidden" r:id="rId7"/>
+    <sheet name="_versioning" sheetId="9" r:id="rId2"/>
+    <sheet name="_issue_tracking" sheetId="7" r:id="rId3"/>
+    <sheet name="_carb_only" sheetId="2" r:id="rId4"/>
+    <sheet name="_json_schema" sheetId="3" r:id="rId5"/>
+    <sheet name="_json_metadata" sheetId="4" r:id="rId6"/>
+    <sheet name="_named_ranges" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="jinja_able_to_repair">'Feedback Form'!$D$51</definedName>
@@ -3771,8 +3770,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4809,7 +4808,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="L5MN8ZoR3m1n6Eqeb+9tGbiq4MU+OigOIODWOwph+cQFuQ1fqCNDRs6GgQoe+Pqg0J1RnwdgPKbmbl0dtK+ThA==" saltValue="B63g8yceyf9mrSlvBCecbA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -7583,7 +7581,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>